<commit_message>
commit changes to excel parsing and dynamic path
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2775" windowWidth="15210" windowHeight="6165" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2775" windowWidth="15210" windowHeight="6165"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -497,7 +497,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -605,7 +605,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>